<commit_message>
file show work done
</commit_message>
<xml_diff>
--- a/dummy_data/week1.xlsx
+++ b/dummy_data/week1.xlsx
@@ -1,26 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26215"/>
-  <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/SSD/htdocs/tms/dummy_data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="22260" windowHeight="12640"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -143,7 +138,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -487,16 +482,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:AH27"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -600,7 +596,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -705,7 +701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -810,7 +806,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -915,7 +911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
@@ -1020,7 +1016,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
@@ -1125,7 +1121,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
@@ -1230,7 +1226,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +1331,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -1440,7 +1436,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
@@ -1545,7 +1541,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1650,7 +1646,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
@@ -1755,7 +1751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -1860,7 +1856,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
@@ -1965,7 +1961,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -2070,7 +2066,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2175,7 +2171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
@@ -2280,7 +2276,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
@@ -2385,7 +2381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
@@ -2490,7 +2486,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
@@ -2595,7 +2591,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2700,7 +2696,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
@@ -2803,7 +2799,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
@@ -2908,7 +2904,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
@@ -3013,7 +3009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
@@ -3118,7 +3114,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
@@ -3223,7 +3219,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>